<commit_message>
adjust for difference instance
</commit_message>
<xml_diff>
--- a/data/instance/100/schedule_1.xlsx
+++ b/data/instance/100/schedule_1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
+    <numFmt formatCode="[hh]:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -46,16 +46,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -402,20 +402,18 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>JQ117</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.1993055555555556</v>
+        <v>0.02569444444444444</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.05138888888888889</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>D36</t>
+          <t>F57</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -432,24 +430,22 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BS308</t>
-        </is>
+      <c r="B3" t="n">
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.2027777777777778</v>
+        <v>0.03680555555555556</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.2256944444444444</v>
+        <v>0.06111111111111111</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A18</t>
+          <t>D31</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -462,20 +458,18 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>6E58S</t>
-        </is>
+      <c r="B4" t="n">
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0.20625</v>
+        <v>0.03680555555555556</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>F40</t>
+          <t>E21</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -492,20 +486,18 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TR892</t>
-        </is>
+      <c r="B5" t="n">
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0.2125</v>
+        <v>0.004861111111111111</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.03125</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>C24</t>
+          <t>E2</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -522,24 +514,22 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>6E54S</t>
-        </is>
+      <c r="B6" t="n">
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.01875</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.2430555555555556</v>
+        <v>0.04097222222222222</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>F33</t>
+          <t>C21</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -552,24 +542,22 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3K761</t>
-        </is>
+      <c r="B7" t="n">
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0.2465277777777778</v>
+        <v>0.04583333333333333</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.2673611111111111</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>D40</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -582,20 +570,18 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NH802</t>
-        </is>
+      <c r="B8" t="n">
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0.2506944444444444</v>
+        <v>0.06736111111111111</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.2743055555555556</v>
+        <v>0.09375</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>F54</t>
+          <t>E22</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -612,24 +598,22 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SQ950</t>
-        </is>
+      <c r="B9" t="n">
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0.2611111111111111</v>
+        <v>0.06458333333333334</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0.2847222222222222</v>
+        <v>0.08611111111111111</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>F60</t>
+          <t>A5</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -642,20 +626,18 @@
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>MI176</t>
-        </is>
+      <c r="B10" t="n">
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0.2652777777777778</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0.2881944444444444</v>
+        <v>0.1020833333333333</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>F52</t>
+          <t>D37</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -672,20 +654,18 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>TR688</t>
-        </is>
+      <c r="B11" t="n">
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0.2645833333333333</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.2881944444444444</v>
+        <v>0.07430555555555556</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>D45</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -702,24 +682,22 @@
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>TR894</t>
-        </is>
+      <c r="B12" t="n">
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0.2673611111111111</v>
+        <v>0.06458333333333334</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.2881944444444444</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>C17</t>
+          <t>E10</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -732,20 +710,18 @@
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>MI436</t>
-        </is>
+      <c r="B13" t="n">
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0.2708333333333333</v>
+        <v>0.05416666666666667</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.08125</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>E2</t>
+          <t>A10</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -762,24 +738,22 @@
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>MI750</t>
-        </is>
+      <c r="B14" t="n">
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0.2680555555555555</v>
+        <v>0.08194444444444444</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.1055555555555556</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>F56</t>
+          <t>C11</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -792,24 +766,22 @@
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>TR608</t>
-        </is>
+      <c r="B15" t="n">
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>0.2680555555555555</v>
+        <v>0.06875000000000001</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.09166666666666666</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>D46</t>
+          <t>C23</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -822,24 +794,22 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>3K243</t>
-        </is>
+      <c r="B16" t="n">
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>0.2722222222222222</v>
+        <v>0.07013888888888889</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>0.2951388888888889</v>
+        <v>0.09375</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>D37</t>
+          <t>C12</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -852,24 +822,22 @@
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SQ241</t>
-        </is>
+      <c r="B17" t="n">
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>0.2743055555555556</v>
+        <v>0.04722222222222222</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0.2951388888888889</v>
+        <v>0.06944444444444445</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>E1</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -882,24 +850,22 @@
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>3K511</t>
-        </is>
+      <c r="B18" t="n">
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>0.2777777777777778</v>
+        <v>0.08055555555555556</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>0.2986111111111111</v>
+        <v>0.1048611111111111</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>D40</t>
+          <t>A12</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -912,20 +878,18 @@
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>3K555</t>
-        </is>
+      <c r="B19" t="n">
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0.2777777777777778</v>
+        <v>0.06597222222222222</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0.2986111111111111</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>C18</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -942,24 +906,22 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>3K721</t>
-        </is>
+      <c r="B20" t="n">
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>0.2777777777777778</v>
+        <v>0.06597222222222222</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.2986111111111111</v>
+        <v>0.08819444444444445</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>C12</t>
+          <t>B5</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -972,20 +934,18 @@
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SQ265</t>
-        </is>
+      <c r="B21" t="n">
+        <v>20</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0.2791666666666667</v>
+        <v>0.04722222222222222</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>0.3020833333333333</v>
+        <v>0.07361111111111111</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>C22</t>
+          <t>A8</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1002,20 +962,18 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>SQ970</t>
-        </is>
+      <c r="B22" t="n">
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>0.28125</v>
+        <v>0.06527777777777778</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0.3020833333333333</v>
+        <v>0.09236111111111112</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>E20</t>
+          <t>F60</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1032,24 +990,22 @@
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>TR280</t>
-        </is>
+      <c r="B23" t="n">
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>0.28125</v>
+        <v>0.06458333333333334</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>0.3020833333333333</v>
+        <v>0.08680555555555555</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>D34</t>
+          <t>A18</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1062,24 +1018,22 @@
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>TR484</t>
-        </is>
+      <c r="B24" t="n">
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>0.2784722222222222</v>
+        <v>0.07569444444444444</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>0.3020833333333333</v>
+        <v>0.09791666666666667</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>D43</t>
+          <t>F41</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1092,20 +1046,18 @@
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>3K683</t>
-        </is>
+      <c r="B25" t="n">
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>0.2826388888888889</v>
+        <v>0.09444444444444444</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>0.3055555555555556</v>
+        <v>0.1173611111111111</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>C19</t>
+          <t>F35</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1122,24 +1074,22 @@
       <c r="A26" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>TR304</t>
-        </is>
+      <c r="B26" t="n">
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>0.2881944444444444</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>0.3090277777777778</v>
+        <v>0.1055555555555556</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>C13</t>
+          <t>E20</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1152,20 +1102,18 @@
       <c r="A27" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>MI234</t>
-        </is>
+      <c r="B27" t="n">
+        <v>26</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.1</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>0.3125</v>
+        <v>0.1215277777777778</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>F37</t>
+          <t>C24</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1182,24 +1130,22 @@
       <c r="A28" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>MI602</t>
-        </is>
+      <c r="B28" t="n">
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>0.2986111111111111</v>
+        <v>0.1097222222222222</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>0.3194444444444444</v>
+        <v>0.13125</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>F32</t>
+          <t>A7</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1212,24 +1158,22 @@
       <c r="A29" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>SQ213</t>
-        </is>
+      <c r="B29" t="n">
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>0.2958333333333333</v>
+        <v>0.09930555555555555</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>0.3194444444444444</v>
+        <v>0.1243055555555556</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>E5</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1242,24 +1186,22 @@
       <c r="A30" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>SQ952</t>
-        </is>
+      <c r="B30" t="n">
+        <v>29</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>0.2986111111111111</v>
+        <v>0.09097222222222222</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>0.3194444444444444</v>
+        <v>0.1159722222222222</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>F41</t>
+          <t>F42</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1272,20 +1214,18 @@
       <c r="A31" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>TR264</t>
-        </is>
+      <c r="B31" t="n">
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>0.2965277777777778</v>
+        <v>0.09861111111111111</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>0.3194444444444444</v>
+        <v>0.1236111111111111</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>D32</t>
+          <t>D45</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1302,24 +1242,22 @@
       <c r="A32" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>3K201</t>
-        </is>
+      <c r="B32" t="n">
+        <v>31</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>0.2993055555555555</v>
+        <v>0.08472222222222223</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>0.3229166666666667</v>
+        <v>0.1055555555555556</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>D38</t>
+          <t>A19</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1332,20 +1270,18 @@
       <c r="A33" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>SQ207</t>
-        </is>
+      <c r="B33" t="n">
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>0.2993055555555555</v>
+        <v>0.1</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>0.3229166666666667</v>
+        <v>0.1215277777777778</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>A15</t>
+          <t>B8</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1362,24 +1298,22 @@
       <c r="A34" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>SQ422</t>
-        </is>
+      <c r="B34" t="n">
+        <v>33</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>0.3</v>
+        <v>0.1215277777777778</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>0.3229166666666667</v>
+        <v>0.14375</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>A12</t>
+          <t>E22</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -1392,24 +1326,22 @@
       <c r="A35" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>SQ930</t>
-        </is>
+      <c r="B35" t="n">
+        <v>34</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>0.3055555555555556</v>
+        <v>0.08819444444444445</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>0.3263888888888889</v>
+        <v>0.1138888888888889</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>F59</t>
+          <t>F50</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -1422,24 +1354,22 @@
       <c r="A36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>3K533</t>
-        </is>
+      <c r="B36" t="n">
+        <v>35</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>0.3069444444444445</v>
+        <v>0.09444444444444444</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>0.3298611111111111</v>
+        <v>0.1159722222222222</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>C17</t>
+          <t>D44</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -1452,24 +1382,22 @@
       <c r="A37" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>SQ998</t>
-        </is>
+      <c r="B37" t="n">
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>0.30625</v>
+        <v>0.1222222222222222</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>0.3298611111111111</v>
+        <v>0.1444444444444444</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>F50</t>
+          <t>E25</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -1482,24 +1410,22 @@
       <c r="A38" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>TR426</t>
-        </is>
+      <c r="B38" t="n">
+        <v>37</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>0.3104166666666667</v>
+        <v>0.1222222222222222</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1444444444444444</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>C16</t>
+          <t>C22</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -1512,20 +1438,18 @@
       <c r="A39" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>SQ600</t>
-        </is>
+      <c r="B39" t="n">
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>0.3138888888888889</v>
+        <v>0.08819444444444445</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>0.3368055555555556</v>
+        <v>0.1138888888888889</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>E26</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1542,24 +1466,22 @@
       <c r="A40" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>SQ632</t>
-        </is>
+      <c r="B40" t="n">
+        <v>39</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>0.3138888888888889</v>
+        <v>0.08541666666666667</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>0.3368055555555556</v>
+        <v>0.1097222222222222</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>A17</t>
+          <t>D36</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -1572,24 +1494,22 @@
       <c r="A41" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>MI772</t>
-        </is>
+      <c r="B41" t="n">
+        <v>40</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>0.3173611111111111</v>
+        <v>0.1159722222222222</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>0.3402777777777778</v>
+        <v>0.1402777777777778</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>E10</t>
+          <t>F36</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -1602,24 +1522,22 @@
       <c r="A42" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>AI381</t>
-        </is>
+      <c r="B42" t="n">
+        <v>41</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>0.3263888888888889</v>
+        <v>0.1631944444444444</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>0.3472222222222222</v>
+        <v>0.1861111111111111</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>F33</t>
+          <t>C17</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
@@ -1632,24 +1550,22 @@
       <c r="A43" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>JL712</t>
-        </is>
+      <c r="B43" t="n">
+        <v>42</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>0.3243055555555556</v>
+        <v>0.1631944444444444</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>0.3472222222222222</v>
+        <v>0.1840277777777778</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>C24</t>
+          <t>F53</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -1662,20 +1578,18 @@
       <c r="A44" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>SQ36S</t>
-        </is>
+      <c r="B44" t="n">
+        <v>43</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>0.3243055555555556</v>
+        <v>0.1513888888888889</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>0.3472222222222222</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>B10</t>
+          <t>D31</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1692,24 +1606,22 @@
       <c r="A45" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>SQ938</t>
-        </is>
+      <c r="B45" t="n">
+        <v>44</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>0.3243055555555556</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>0.3472222222222222</v>
+        <v>0.1625</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>F40</t>
+          <t>F34</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -1722,24 +1634,22 @@
       <c r="A46" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>TR384</t>
-        </is>
+      <c r="B46" t="n">
+        <v>45</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>0.3236111111111111</v>
+        <v>0.1347222222222222</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>0.3472222222222222</v>
+        <v>0.1569444444444444</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>D43</t>
+          <t>A15</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -1752,24 +1662,22 @@
       <c r="A47" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>SQ620</t>
-        </is>
+      <c r="B47" t="n">
+        <v>46</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>0.3277777777777778</v>
+        <v>0.1604166666666667</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>0.3506944444444444</v>
+        <v>0.1833333333333333</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>A16</t>
+          <t>B8</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
@@ -1782,24 +1690,22 @@
       <c r="A48" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>MI324</t>
-        </is>
+      <c r="B48" t="n">
+        <v>47</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>0.3541666666666667</v>
+        <v>0.16875</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>F52</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -1812,24 +1718,22 @@
       <c r="A49" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>TR648</t>
-        </is>
+      <c r="B49" t="n">
+        <v>48</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>0.3305555555555555</v>
+        <v>0.1381944444444445</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>0.3541666666666667</v>
+        <v>0.1645833333333333</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>D35</t>
+          <t>D46</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
@@ -1842,24 +1746,22 @@
       <c r="A50" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>TR874</t>
-        </is>
+      <c r="B50" t="n">
+        <v>49</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>0.33125</v>
+        <v>0.1493055555555556</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>0.3541666666666667</v>
+        <v>0.1729166666666667</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>C11</t>
+          <t>D42</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
@@ -1872,20 +1774,18 @@
       <c r="A51" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>CA404</t>
-        </is>
+      <c r="B51" t="n">
+        <v>50</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>0.3402777777777778</v>
+        <v>0.1284722222222222</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1555555555555556</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>D44</t>
+          <t>E1</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -1902,24 +1802,22 @@
       <c r="A52" t="n">
         <v>51</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>MI614</t>
-        </is>
+      <c r="B52" t="n">
+        <v>51</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>0.3402777777777778</v>
+        <v>0.1263888888888889</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1527777777777778</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>F56</t>
+          <t>A17</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -1932,24 +1830,22 @@
       <c r="A53" t="n">
         <v>52</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>MI801</t>
-        </is>
+      <c r="B53" t="n">
+        <v>52</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>0.3381944444444445</v>
+        <v>0.1340277777777778</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1604166666666667</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>F35</t>
+          <t>F37</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
@@ -1962,20 +1858,18 @@
       <c r="A54" t="n">
         <v>53</v>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>MI813</t>
-        </is>
+      <c r="B54" t="n">
+        <v>53</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>0.3375</v>
+        <v>0.15</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1722222222222222</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>E7</t>
+          <t>E11</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -1992,20 +1886,18 @@
       <c r="A55" t="n">
         <v>54</v>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>SQ182</t>
-        </is>
+      <c r="B55" t="n">
+        <v>54</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>0.3381944444444445</v>
+        <v>0.1409722222222222</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1631944444444444</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>E1</t>
+          <t>C1</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2022,20 +1914,18 @@
       <c r="A56" t="n">
         <v>55</v>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>SQ281</t>
-        </is>
+      <c r="B56" t="n">
+        <v>55</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>0.3416666666666667</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>0.3645833333333333</v>
+        <v>0.1708333333333333</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>A13</t>
+          <t>D49</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2052,20 +1942,18 @@
       <c r="A57" t="n">
         <v>56</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>SQ802</t>
-        </is>
+      <c r="B57" t="n">
+        <v>56</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>0.3506944444444444</v>
+        <v>0.1611111111111111</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>0.3715277777777778</v>
+        <v>0.1881944444444444</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>B5</t>
+          <t>D48</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2082,24 +1970,22 @@
       <c r="A58" t="n">
         <v>57</v>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>AI347</t>
-        </is>
+      <c r="B58" t="n">
+        <v>57</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>0.3520833333333334</v>
+        <v>0.1534722222222222</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>0.375</v>
+        <v>0.1805555555555556</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>F33</t>
+          <t>C26</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -2112,24 +1998,22 @@
       <c r="A59" t="n">
         <v>58</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>SQ308</t>
-        </is>
+      <c r="B59" t="n">
+        <v>58</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>0.3520833333333334</v>
+        <v>0.1743055555555555</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>0.375</v>
+        <v>0.2013888888888889</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A18</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -2142,24 +2026,22 @@
       <c r="A60" t="n">
         <v>59</v>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>MI424</t>
-        </is>
+      <c r="B60" t="n">
+        <v>59</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>0.3548611111111111</v>
+        <v>0.1798611111111111</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>0.3784722222222222</v>
+        <v>0.2013888888888889</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>F35</t>
+          <t>C23</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" t="n">
         <v>0</v>
@@ -2172,24 +2054,22 @@
       <c r="A61" t="n">
         <v>60</v>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>SQ942</t>
-        </is>
+      <c r="B61" t="n">
+        <v>60</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>0.3576388888888889</v>
+        <v>0.2006944444444445</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>0.3784722222222222</v>
+        <v>0.2215277777777778</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>F31</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -2202,20 +2082,18 @@
       <c r="A62" t="n">
         <v>61</v>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>3K581</t>
-        </is>
+      <c r="B62" t="n">
+        <v>61</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1875</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>0.3819444444444444</v>
+        <v>0.2118055555555556</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>D30</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="F62" t="n">
@@ -2232,24 +2110,22 @@
       <c r="A63" t="n">
         <v>62</v>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>TR300</t>
-        </is>
+      <c r="B63" t="n">
+        <v>62</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>0.3583333333333333</v>
+        <v>0.175</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>0.3819444444444444</v>
+        <v>0.2</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>C3</t>
+          <t>E8</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
@@ -2262,24 +2138,22 @@
       <c r="A64" t="n">
         <v>63</v>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>TR452</t>
-        </is>
+      <c r="B64" t="n">
+        <v>63</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>0.3611111111111111</v>
+        <v>0.1951388888888889</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>0.3819444444444444</v>
+        <v>0.2159722222222222</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>D42</t>
+          <t>F51</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
@@ -2292,24 +2166,22 @@
       <c r="A65" t="n">
         <v>64</v>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>MI632</t>
-        </is>
+      <c r="B65" t="n">
+        <v>64</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>0.3645833333333333</v>
+        <v>0.1756944444444444</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>0.3854166666666667</v>
+        <v>0.1972222222222222</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>F56</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2322,20 +2194,18 @@
       <c r="A66" t="n">
         <v>65</v>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>SQ176</t>
-        </is>
+      <c r="B66" t="n">
+        <v>65</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>0.3625</v>
+        <v>0.2069444444444444</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>0.3854166666666667</v>
+        <v>0.2305555555555556</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>E24</t>
+          <t>B6</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -2352,24 +2222,22 @@
       <c r="A67" t="n">
         <v>66</v>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>SQ910</t>
-        </is>
+      <c r="B67" t="n">
+        <v>66</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>0.3625</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>0.3854166666666667</v>
+        <v>0.2006944444444445</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>E12</t>
+          <t>F60</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
@@ -2382,20 +2250,18 @@
       <c r="A68" t="n">
         <v>67</v>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>SQ12S</t>
-        </is>
+      <c r="B68" t="n">
+        <v>67</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>0.3680555555555556</v>
+        <v>0.2048611111111111</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>0.3888888888888889</v>
+        <v>0.2319444444444445</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -2412,20 +2278,18 @@
       <c r="A69" t="n">
         <v>68</v>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>SQ32S</t>
-        </is>
+      <c r="B69" t="n">
+        <v>68</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>0.3659722222222222</v>
+        <v>0.175</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>0.3888888888888889</v>
+        <v>0.1972222222222222</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>C25</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -2442,20 +2306,18 @@
       <c r="A70" t="n">
         <v>69</v>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>SQ830</t>
-        </is>
+      <c r="B70" t="n">
+        <v>69</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>0.3659722222222222</v>
+        <v>0.2444444444444444</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>0.3888888888888889</v>
+        <v>0.2659722222222222</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>B8</t>
+          <t>D31</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -2472,24 +2334,22 @@
       <c r="A71" t="n">
         <v>70</v>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>SQ28S</t>
-        </is>
+      <c r="B71" t="n">
+        <v>70</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>0.3715277777777778</v>
+        <v>0.2381944444444444</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>0.3923611111111111</v>
+        <v>0.2611111111111111</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>B9</t>
+          <t>D35</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G71" t="n">
         <v>0</v>
@@ -2502,20 +2362,18 @@
       <c r="A72" t="n">
         <v>71</v>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>3K663</t>
-        </is>
+      <c r="B72" t="n">
+        <v>71</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>0.3729166666666667</v>
+        <v>0.2270833333333333</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.2527777777777778</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>C12</t>
+          <t>E11</t>
         </is>
       </c>
       <c r="F72" t="n">
@@ -2532,20 +2390,18 @@
       <c r="A73" t="n">
         <v>72</v>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>SQ223</t>
-        </is>
+      <c r="B73" t="n">
+        <v>72</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>0.375</v>
+        <v>0.2152777777777778</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.2388888888888889</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>F30</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -2562,24 +2418,22 @@
       <c r="A74" t="n">
         <v>73</v>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>SQ956</t>
-        </is>
+      <c r="B74" t="n">
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>0.3722222222222222</v>
+        <v>0.2270833333333333</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.2527777777777778</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>E11</t>
+          <t>C19</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
@@ -2592,24 +2446,22 @@
       <c r="A75" t="n">
         <v>74</v>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>TR606</t>
-        </is>
+      <c r="B75" t="n">
+        <v>74</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>0.375</v>
+        <v>0.2284722222222222</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.2541666666666667</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>D41</t>
+          <t>F36</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G75" t="n">
         <v>0</v>
@@ -2622,24 +2474,22 @@
       <c r="A76" t="n">
         <v>75</v>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>UK116</t>
-        </is>
+      <c r="B76" t="n">
+        <v>75</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>0.3722222222222222</v>
+        <v>0.2354166666666667</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.2597222222222222</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>A7</t>
+          <t>C3</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G76" t="n">
         <v>0</v>
@@ -2652,20 +2502,18 @@
       <c r="A77" t="n">
         <v>76</v>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>EK433</t>
-        </is>
+      <c r="B77" t="n">
+        <v>76</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>0.3763888888888889</v>
+        <v>0.2256944444444444</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>0.3993055555555556</v>
+        <v>0.2520833333333333</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>C13</t>
+          <t>A7</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -2682,24 +2530,22 @@
       <c r="A78" t="n">
         <v>77</v>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>SQ288</t>
-        </is>
+      <c r="B78" t="n">
+        <v>77</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>0.3763888888888889</v>
+        <v>0.2125</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>0.3993055555555556</v>
+        <v>0.2347222222222222</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>A14</t>
+          <t>C26</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G78" t="n">
         <v>0</v>
@@ -2712,24 +2558,22 @@
       <c r="A79" t="n">
         <v>78</v>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>JT153</t>
-        </is>
+      <c r="B79" t="n">
+        <v>78</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>0.3854166666666667</v>
+        <v>0.2298611111111111</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>0.40625</v>
+        <v>0.2527777777777778</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>A11</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
@@ -2742,24 +2586,22 @@
       <c r="A80" t="n">
         <v>79</v>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>SQ245</t>
-        </is>
+      <c r="B80" t="n">
+        <v>79</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>0.3826388888888889</v>
+        <v>0.2284722222222222</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>0.40625</v>
+        <v>0.2506944444444444</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A13</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
@@ -2772,20 +2614,18 @@
       <c r="A81" t="n">
         <v>80</v>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>SQ972</t>
-        </is>
+      <c r="B81" t="n">
+        <v>80</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>0.3854166666666667</v>
+        <v>0.2506944444444444</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>0.40625</v>
+        <v>0.2715277777777778</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>F34</t>
+          <t>B5</t>
         </is>
       </c>
       <c r="F81" t="n">
@@ -2802,24 +2642,22 @@
       <c r="A82" t="n">
         <v>81</v>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>UL307</t>
-        </is>
+      <c r="B82" t="n">
+        <v>81</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>0.3833333333333334</v>
+        <v>0.2895833333333334</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>0.40625</v>
+        <v>0.3145833333333333</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>A9</t>
+          <t>E6</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G82" t="n">
         <v>0</v>
@@ -2832,24 +2670,22 @@
       <c r="A83" t="n">
         <v>82</v>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>SQ178</t>
-        </is>
+      <c r="B83" t="n">
+        <v>82</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>0.3861111111111111</v>
+        <v>0.2875</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>0.4097222222222222</v>
+        <v>0.3131944444444444</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>F41</t>
+          <t>D37</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G83" t="n">
         <v>0</v>
@@ -2862,20 +2698,18 @@
       <c r="A84" t="n">
         <v>83</v>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>SQ992</t>
-        </is>
+      <c r="B84" t="n">
+        <v>83</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>0.3868055555555556</v>
+        <v>0.2590277777777778</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>0.4097222222222222</v>
+        <v>0.28125</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>E22</t>
+          <t>F36</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -2892,20 +2726,18 @@
       <c r="A85" t="n">
         <v>84</v>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>TR276</t>
-        </is>
+      <c r="B85" t="n">
+        <v>84</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>0.3861111111111111</v>
+        <v>0.2548611111111111</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>0.4097222222222222</v>
+        <v>0.28125</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>C18</t>
+          <t>B9</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -2922,24 +2754,22 @@
       <c r="A86" t="n">
         <v>85</v>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>MH604</t>
-        </is>
+      <c r="B86" t="n">
+        <v>85</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>0.3902777777777778</v>
+        <v>0.2604166666666667</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>0.4131944444444444</v>
+        <v>0.2868055555555555</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>F32</t>
+          <t>E20</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G86" t="n">
         <v>0</v>
@@ -2952,20 +2782,18 @@
       <c r="A87" t="n">
         <v>86</v>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>SQ856</t>
-        </is>
+      <c r="B87" t="n">
+        <v>86</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>0.3923611111111111</v>
+        <v>0.2680555555555555</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>0.4131944444444444</v>
+        <v>0.2944444444444445</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>A12</t>
+          <t>A18</t>
         </is>
       </c>
       <c r="F87" t="n">
@@ -2982,24 +2810,22 @@
       <c r="A88" t="n">
         <v>87</v>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>GA825</t>
-        </is>
+      <c r="B88" t="n">
+        <v>87</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>0.39375</v>
+        <v>0.2868055555555555</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.3118055555555556</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>A17</t>
+          <t>E24</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G88" t="n">
         <v>0</v>
@@ -3012,24 +2838,22 @@
       <c r="A89" t="n">
         <v>88</v>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>MI348</t>
-        </is>
+      <c r="B89" t="n">
+        <v>88</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.2819444444444444</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.3048611111111111</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>F37</t>
+          <t>D35</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G89" t="n">
         <v>0</v>
@@ -3042,24 +2866,22 @@
       <c r="A90" t="n">
         <v>89</v>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>MI194</t>
-        </is>
+      <c r="B90" t="n">
+        <v>89</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>0.3965277777777778</v>
+        <v>0.2868055555555555</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>0.4201388888888889</v>
+        <v>0.3097222222222222</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>E2</t>
+          <t>D31</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G90" t="n">
         <v>0</v>
@@ -3072,20 +2894,18 @@
       <c r="A91" t="n">
         <v>90</v>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>MI482</t>
-        </is>
+      <c r="B91" t="n">
+        <v>90</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>0.3972222222222222</v>
+        <v>0.26875</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>0.4201388888888889</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>F52</t>
+          <t>F59</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -3102,24 +2922,22 @@
       <c r="A92" t="n">
         <v>91</v>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>EK432</t>
-        </is>
+      <c r="B92" t="n">
+        <v>91</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>0.4027777777777778</v>
+        <v>0.3097222222222222</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.3368055555555556</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>C23</t>
+          <t>C20</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G92" t="n">
         <v>0</v>
@@ -3132,24 +2950,22 @@
       <c r="A93" t="n">
         <v>92</v>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>OD802</t>
-        </is>
+      <c r="B93" t="n">
+        <v>92</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>0.4006944444444445</v>
+        <v>0.3180555555555555</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>A16</t>
+          <t>D36</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G93" t="n">
         <v>0</v>
@@ -3162,24 +2978,22 @@
       <c r="A94" t="n">
         <v>93</v>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>UA2SI</t>
-        </is>
+      <c r="B94" t="n">
+        <v>93</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>0.4</v>
+        <v>0.3263888888888889</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.3527777777777778</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>F54</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G94" t="n">
         <v>0</v>
@@ -3192,24 +3006,22 @@
       <c r="A95" t="n">
         <v>94</v>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>3K281</t>
-        </is>
+      <c r="B95" t="n">
+        <v>94</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>0.4041666666666667</v>
+        <v>0.2958333333333333</v>
       </c>
       <c r="D95" s="1" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.3201388888888889</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>D40</t>
+          <t>E28</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G95" t="n">
         <v>0</v>
@@ -3222,24 +3034,22 @@
       <c r="A96" t="n">
         <v>95</v>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>MI326</t>
-        </is>
+      <c r="B96" t="n">
+        <v>95</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>0.40625</v>
+        <v>0.3104166666666667</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>F30</t>
+          <t>D38</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G96" t="n">
         <v>0</v>
@@ -3252,20 +3062,18 @@
       <c r="A97" t="n">
         <v>96</v>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>TR454</t>
-        </is>
+      <c r="B97" t="n">
+        <v>96</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>0.4041666666666667</v>
+        <v>0.3145833333333333</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.3388888888888889</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>C17</t>
+          <t>A18</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -3282,24 +3090,22 @@
       <c r="A98" t="n">
         <v>97</v>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>TR470</t>
-        </is>
+      <c r="B98" t="n">
+        <v>97</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>0.40625</v>
+        <v>0.3506944444444444</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.3777777777777778</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>C26</t>
+          <t>E12</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G98" t="n">
         <v>0</v>
@@ -3312,20 +3118,18 @@
       <c r="A99" t="n">
         <v>98</v>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>CI752</t>
-        </is>
+      <c r="B99" t="n">
+        <v>98</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>0.4104166666666667</v>
+        <v>0.3381944444444445</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>0.4340277777777778</v>
+        <v>0.3590277777777778</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>F33</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -3342,20 +3146,18 @@
       <c r="A100" t="n">
         <v>99</v>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>SQ211</t>
-        </is>
+      <c r="B100" t="n">
+        <v>99</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>0.4145833333333334</v>
+        <v>0.36875</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>0.4375</v>
+        <v>0.3930555555555555</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>D41</t>
         </is>
       </c>
       <c r="F100" t="n">
@@ -3372,24 +3174,22 @@
       <c r="A101" t="n">
         <v>100</v>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>TR284</t>
-        </is>
+      <c r="B101" t="n">
+        <v>100</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>0.4138888888888889</v>
+        <v>0.3423611111111111</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>0.4375</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>D40</t>
+          <t>C23</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G101" t="n">
         <v>0</v>
@@ -3399,6 +3199,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>